<commit_message>
FY_ constants moved to fy_constants.py; new module fy_ratios with several company-related ratios; invesement_reading: getRiskM for risk matrix added
</commit_message>
<xml_diff>
--- a/FY mapping.xlsx
+++ b/FY mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankifor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankifor\Desktop\IDP\IDP_Risks_Assesment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -544,7 +544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -552,7 +554,7 @@
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="47.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -586,16 +588,16 @@
         <v>60</v>
       </c>
       <c r="D2" t="str">
-        <f>UPPER($D$1&amp;"_"&amp;C2)</f>
-        <v>FY_ID</v>
+        <f>UPPER($D$1&amp;"."&amp;C2)</f>
+        <v>FY.ID</v>
       </c>
       <c r="E2" t="str">
         <f>$E$1&amp;"['"&amp;A2&amp;"'] = "&amp;D2</f>
-        <v>remapCols['ID'] = FY_ID</v>
+        <v>remapCols['ID'] = FY.ID</v>
       </c>
       <c r="F2" t="str">
-        <f>D2&amp;" = '" &amp;B2&amp;"'"</f>
-        <v>FY_ID = 'ID'</v>
+        <f>UPPER(C2)&amp;" = '" &amp;B2&amp;"'"</f>
+        <v>ID = 'ID'</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,16 +611,16 @@
         <v>61</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D24" si="0">UPPER($D$1&amp;"_"&amp;C3)</f>
-        <v>FY_YEAR</v>
+        <f t="shared" ref="D3:D24" si="0">UPPER($D$1&amp;"."&amp;C3)</f>
+        <v>FY.YEAR</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E24" si="1">$E$1&amp;"['"&amp;A3&amp;"'] = "&amp;D3</f>
-        <v>remapCols['Year'] = FY_YEAR</v>
+        <v>remapCols['Year'] = FY.YEAR</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F24" si="2">D3&amp;" = '" &amp;B3&amp;"'"</f>
-        <v>FY_YEAR = 'Year'</v>
+        <f t="shared" ref="F3:F24" si="2">UPPER(C3)&amp;" = '" &amp;B3&amp;"'"</f>
+        <v>YEAR = 'Year'</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -633,15 +635,15 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>FY_ISIN</v>
+        <v>FY.ISIN</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['ISIN'] = FY_ISIN</v>
+        <v>remapCols['ISIN'] = FY.ISIN</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
-        <v>FY_ISIN = 'ISIN'</v>
+        <v>ISIN = 'ISIN'</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,15 +658,15 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>FY_EBITDA</v>
+        <v>FY.EBITDA</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Normalized EBITDA'] = FY_EBITDA</v>
+        <v>remapCols['Normalized EBITDA'] = FY.EBITDA</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
-        <v>FY_EBITDA = 'EBITDA'</v>
+        <v>EBITDA = 'EBITDA'</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -679,15 +681,15 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>FY_EBIT</v>
+        <v>FY.EBIT</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Normalized EBIT'] = FY_EBIT</v>
+        <v>remapCols['Normalized EBIT'] = FY.EBIT</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>FY_EBIT = 'EBIT'</v>
+        <v>EBIT = 'EBIT'</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,15 +704,15 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>FY_EBT</v>
+        <v>FY.EBT</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Normalized Income Before Taxes'] = FY_EBT</v>
+        <v>remapCols['Normalized Income Before Taxes'] = FY.EBT</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>FY_EBT = 'EBT'</v>
+        <v>EBT = 'EBT'</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -725,15 +727,15 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>FY_NET_INCOME</v>
+        <v>FY.NET_INCOME</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Normalized Income After Taxes'] = FY_NET_INCOME</v>
+        <v>remapCols['Normalized Income After Taxes'] = FY.NET_INCOME</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>FY_NET_INCOME = 'Net Income'</v>
+        <v>NET_INCOME = 'Net Income'</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,15 +750,15 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_REVENUE</v>
+        <v>FY.TOT_REVENUE</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Revenue'] = FY_TOT_REVENUE</v>
+        <v>remapCols['Total Revenue'] = FY.TOT_REVENUE</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_REVENUE = 'Tot Revenue'</v>
+        <v>TOT_REVENUE = 'Tot Revenue'</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,15 +773,15 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_DEBT</v>
+        <v>FY.TOT_DEBT</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Debt'] = FY_TOT_DEBT</v>
+        <v>remapCols['Total Debt'] = FY.TOT_DEBT</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_DEBT = 'Tot Debt'</v>
+        <v>TOT_DEBT = 'Tot Debt'</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,15 +796,15 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>FY_ACC_RECEIVABLE</v>
+        <v>FY.ACC_RECEIVABLE</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Accounts Receivable - Trade, Net'] = FY_ACC_RECEIVABLE</v>
+        <v>remapCols['Accounts Receivable - Trade, Net'] = FY.ACC_RECEIVABLE</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>FY_ACC_RECEIVABLE = 'Acc Receivable'</v>
+        <v>ACC_RECEIVABLE = 'Acc Receivable'</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -817,15 +819,15 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>FY_ACC_PAYABLE</v>
+        <v>FY.ACC_PAYABLE</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Accounts Payable'] = FY_ACC_PAYABLE</v>
+        <v>remapCols['Accounts Payable'] = FY.ACC_PAYABLE</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>FY_ACC_PAYABLE = 'Acc Payable'</v>
+        <v>ACC_PAYABLE = 'Acc Payable'</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,15 +842,15 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_INVENTORY</v>
+        <v>FY.TOT_INVENTORY</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Inventory'] = FY_TOT_INVENTORY</v>
+        <v>remapCols['Total Inventory'] = FY.TOT_INVENTORY</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_INVENTORY = 'Tot Inventory'</v>
+        <v>TOT_INVENTORY = 'Tot Inventory'</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,15 +865,15 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>FY_COGS</v>
+        <v>FY.COGS</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Cost Of Goods Sold - Actual'] = FY_COGS</v>
+        <v>remapCols['Cost Of Goods Sold - Actual'] = FY.COGS</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>FY_COGS = 'COGS'</v>
+        <v>COGS = 'COGS'</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -886,15 +888,15 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>FY_ENTERPR_VALUE</v>
+        <v>FY.ENTERPR_VALUE</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Enterprise Value (Daily Time Series)'] = FY_ENTERPR_VALUE</v>
+        <v>remapCols['Enterprise Value (Daily Time Series)'] = FY.ENTERPR_VALUE</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
-        <v>FY_ENTERPR_VALUE = 'Enterpr Value'</v>
+        <v>ENTERPR_VALUE = 'Enterpr Value'</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,15 +911,15 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>FY_NET_DEBT</v>
+        <v>FY.NET_DEBT</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Net Debt - Mean'] = FY_NET_DEBT</v>
+        <v>remapCols['Net Debt - Mean'] = FY.NET_DEBT</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
-        <v>FY_NET_DEBT = 'Net Debt'</v>
+        <v>NET_DEBT = 'Net Debt'</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,15 +934,15 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_CURR_ASSETS</v>
+        <v>FY.TOT_CURR_ASSETS</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Current Assets'] = FY_TOT_CURR_ASSETS</v>
+        <v>remapCols['Total Current Assets'] = FY.TOT_CURR_ASSETS</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_CURR_ASSETS = 'Tot Curr Assets'</v>
+        <v>TOT_CURR_ASSETS = 'Tot Curr Assets'</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,15 +957,15 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_CURR_LIABILITIES</v>
+        <v>FY.TOT_CURR_LIABILITIES</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Current Liabilities'] = FY_TOT_CURR_LIABILITIES</v>
+        <v>remapCols['Total Current Liabilities'] = FY.TOT_CURR_LIABILITIES</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_CURR_LIABILITIES = 'Tot Curr Liabilities'</v>
+        <v>TOT_CURR_LIABILITIES = 'Tot Curr Liabilities'</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,15 +980,15 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_LIABILITIES</v>
+        <v>FY.TOT_LIABILITIES</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Liabilities'] = FY_TOT_LIABILITIES</v>
+        <v>remapCols['Total Liabilities'] = FY.TOT_LIABILITIES</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_LIABILITIES = 'Tot Liabilities'</v>
+        <v>TOT_LIABILITIES = 'Tot Liabilities'</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,15 +1003,15 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_EQUITY</v>
+        <v>FY.TOT_EQUITY</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Total Equity'] = FY_TOT_EQUITY</v>
+        <v>remapCols['Total Equity'] = FY.TOT_EQUITY</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_EQUITY = 'Tot Equity'</v>
+        <v>TOT_EQUITY = 'Tot Equity'</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,15 +1026,15 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>FY_TOT_COMMON_STOCK</v>
+        <v>FY.TOT_COMMON_STOCK</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Common Stock, Total'] = FY_TOT_COMMON_STOCK</v>
+        <v>remapCols['Common Stock, Total'] = FY.TOT_COMMON_STOCK</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>FY_TOT_COMMON_STOCK = 'Tot Common Stock'</v>
+        <v>TOT_COMMON_STOCK = 'Tot Common Stock'</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,15 +1049,15 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>FY_SHARES_OUT</v>
+        <v>FY.SHARES_OUT</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Shares Out - Common Stock Primary Issue'] = FY_SHARES_OUT</v>
+        <v>remapCols['Shares Out - Common Stock Primary Issue'] = FY.SHARES_OUT</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="2"/>
-        <v>FY_SHARES_OUT = 'Shares Out'</v>
+        <v>SHARES_OUT = 'Shares Out'</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,15 +1072,15 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>FY_CASH_N_EQUIVALENTS</v>
+        <v>FY.CASH_N_EQUIVALENTS</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Cash and Equivalents'] = FY_CASH_N_EQUIVALENTS</v>
+        <v>remapCols['Cash and Equivalents'] = FY.CASH_N_EQUIVALENTS</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>FY_CASH_N_EQUIVALENTS = 'Cash &amp; Equivalents'</v>
+        <v>CASH_N_EQUIVALENTS = 'Cash &amp; Equivalents'</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,15 +1095,15 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>FY_NUM_EMPLOYEES</v>
+        <v>FY.NUM_EMPLOYEES</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>remapCols['Number of Employees'] = FY_NUM_EMPLOYEES</v>
+        <v>remapCols['Number of Employees'] = FY.NUM_EMPLOYEES</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="2"/>
-        <v>FY_NUM_EMPLOYEES = 'Number of Employees'</v>
+        <v>NUM_EMPLOYEES = 'Number of Employees'</v>
       </c>
     </row>
   </sheetData>

</xml_diff>